<commit_message>
Change column names in spreadsheet
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies.xlsx
@@ -29,19 +29,19 @@
     <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t xml:space="preserve">Body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forewing.left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forewing.right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindwing.left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindwing.right</t>
+    <t xml:space="preserve">Body.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forewing.dorsal.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forewing.ventral.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindwing.dorsal.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindwing.ventral.damage</t>
   </si>
   <si>
     <t xml:space="preserve">Site</t>
@@ -65,7 +65,7 @@
     <t xml:space="preserve">Binomial</t>
   </si>
   <si>
-    <t xml:space="preserve">Speced</t>
+    <t xml:space="preserve">Spectra</t>
   </si>
   <si>
     <t xml:space="preserve">DNA</t>

</xml_diff>

<commit_message>
Change .gb to .fastq in test dbs
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies.xlsx
@@ -29,19 +29,22 @@
     <t xml:space="preserve">Sex</t>
   </si>
   <si>
-    <t xml:space="preserve">Body.damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forewing.dorsal.damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forewing.ventral.damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindwing.dorsal.damage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindwing.ventral.damage</t>
+    <t xml:space="preserve">Pinned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Body</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forewing.left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forewing.right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindwing.left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindwing.right</t>
   </si>
   <si>
     <t xml:space="preserve">Site</t>
@@ -65,13 +68,10 @@
     <t xml:space="preserve">Binomial</t>
   </si>
   <si>
+    <t xml:space="preserve">DNA</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spectra</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pinned</t>
   </si>
   <si>
     <t xml:space="preserve">Hesperiidae</t>
@@ -596,31 +596,31 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="n">
+      <c r="M2" t="n">
         <v>-16.90136852</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>145.7505777</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>27</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>30</v>
-      </c>
-      <c r="R2" t="s">
-        <v>25</v>
       </c>
       <c r="S2" t="s">
         <v>24</v>
@@ -661,28 +661,28 @@
         <v>24</v>
       </c>
       <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="L3" t="n">
+      <c r="M3" t="n">
         <v>-16.90136852</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>145.7505777</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>28</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>34</v>
-      </c>
-      <c r="R3" t="s">
-        <v>24</v>
       </c>
       <c r="S3" t="s">
         <v>24</v>
@@ -723,28 +723,28 @@
         <v>24</v>
       </c>
       <c r="K4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="L4" t="n">
+      <c r="M4" t="n">
         <v>-16.90136852</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>145.7505777</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>27</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>28</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>34</v>
-      </c>
-      <c r="R4" t="s">
-        <v>24</v>
       </c>
       <c r="S4" t="s">
         <v>24</v>
@@ -770,11 +770,11 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
         <v>25</v>
       </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
       <c r="H5" t="s">
         <v>24</v>
       </c>
@@ -785,34 +785,34 @@
         <v>24</v>
       </c>
       <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
         <v>37</v>
       </c>
-      <c r="L5" t="n">
+      <c r="M5" t="n">
         <v>-16.81425603</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>145.6854526</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>27</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>28</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>39</v>
-      </c>
-      <c r="R5" t="s">
-        <v>25</v>
       </c>
       <c r="S5" t="s">
         <v>25</v>
       </c>
       <c r="T5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
@@ -832,7 +832,7 @@
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G6" t="s">
         <v>24</v>
@@ -847,28 +847,28 @@
         <v>24</v>
       </c>
       <c r="K6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" t="s">
         <v>43</v>
       </c>
-      <c r="L6" t="n">
+      <c r="M6" t="n">
         <v>-16.45193583</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>145.3714342</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>27</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>44</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>38</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>45</v>
-      </c>
-      <c r="R6" t="s">
-        <v>25</v>
       </c>
       <c r="S6" t="s">
         <v>25</v>
@@ -909,28 +909,28 @@
         <v>24</v>
       </c>
       <c r="K7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" t="s">
         <v>49</v>
       </c>
-      <c r="L7" t="n">
+      <c r="M7" t="n">
         <v>-27.344776</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>153.0390842</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>50</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>51</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>53</v>
-      </c>
-      <c r="R7" t="s">
-        <v>25</v>
       </c>
       <c r="S7" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Zip into genera for storing in repo. Add Repo.zipname column to the specimen metadata spreadsheet.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -74,6 +74,9 @@
     <t xml:space="preserve">Spectra</t>
   </si>
   <si>
+    <t xml:space="preserve">Repo.zipname</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hesperiidae</t>
   </si>
   <si>
@@ -107,6 +110,9 @@
     <t xml:space="preserve">Notocrypta waigensis</t>
   </si>
   <si>
+    <t xml:space="preserve">Hesperiidae_Notocrypta.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Telicota</t>
   </si>
   <si>
@@ -119,6 +125,9 @@
     <t xml:space="preserve">Telicota mesoptis</t>
   </si>
   <si>
+    <t xml:space="preserve">Hesperiidae_Telicota.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suniana</t>
   </si>
   <si>
@@ -134,6 +143,9 @@
     <t xml:space="preserve">Suniana sunias</t>
   </si>
   <si>
+    <t xml:space="preserve">Hesperiidae_Suniana.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nymphalidae</t>
   </si>
   <si>
@@ -152,6 +164,9 @@
     <t xml:space="preserve">Euploea darchia</t>
   </si>
   <si>
+    <t xml:space="preserve">Nymphalidae_Euploea.zip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Papilionidae</t>
   </si>
   <si>
@@ -174,6 +189,9 @@
   </si>
   <si>
     <t xml:space="preserve">Papilio aegeus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Papilionidae_Papilio.zip</t>
   </si>
 </sst>
 </file>
@@ -566,43 +584,46 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M2" t="n">
         <v>-16.90136852</v>
@@ -611,22 +632,25 @@
         <v>145.7505777</v>
       </c>
       <c r="O2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T2" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -634,37 +658,37 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M3" t="n">
         <v>-16.90136852</v>
@@ -673,22 +697,25 @@
         <v>145.7505777</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T3" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="U3" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -696,37 +723,37 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M4" t="n">
         <v>-16.90136852</v>
@@ -735,22 +762,25 @@
         <v>145.7505777</v>
       </c>
       <c r="O4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="S4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="U4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -758,37 +788,37 @@
         <v>186</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M5" t="n">
         <v>-16.81425603</v>
@@ -797,22 +827,25 @@
         <v>145.6854526</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="R5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="S5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T5" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="U5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -820,37 +853,37 @@
         <v>551</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M6" t="n">
         <v>-16.45193583</v>
@@ -859,22 +892,25 @@
         <v>145.3714342</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="Q6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="R6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="S6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T6" t="s">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="U6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -882,37 +918,37 @@
         <v>1361</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L7" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="M7" t="n">
         <v>-27.344776</v>
@@ -921,22 +957,25 @@
         <v>153.0390842</v>
       </c>
       <c r="O7" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="P7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="Q7" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="R7" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="S7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T7" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="U7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix column name error in spreadsheet
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies.xlsx
@@ -32,19 +32,19 @@
     <t xml:space="preserve">Pinned</t>
   </si>
   <si>
-    <t xml:space="preserve">Body</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forewing.left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Forewing.right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindwing.left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hindwing.right</t>
+    <t xml:space="preserve">Body.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forewing.dorsal.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Forewing.ventral.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindwing.dorsal.damage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hindwing.ventral.damage</t>
   </si>
   <si>
     <t xml:space="preserve">Site</t>

</xml_diff>

<commit_message>
Update date format in test data
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies.xlsx
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Tropical</t>
   </si>
   <si>
-    <t xml:space="preserve">16/07/2022</t>
+    <t xml:space="preserve">2022-07-16</t>
   </si>
   <si>
     <t xml:space="preserve">MFE</t>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">MR</t>
   </si>
   <si>
-    <t xml:space="preserve">19/07/2022</t>
+    <t xml:space="preserve">2022-07-19</t>
   </si>
   <si>
     <t xml:space="preserve">Euploea darchia</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">Subtropical</t>
   </si>
   <si>
-    <t xml:space="preserve">24/09/2022</t>
+    <t xml:space="preserve">2022-09-24</t>
   </si>
   <si>
     <t xml:space="preserve">CI</t>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/DiogoJackson/ButtR"
This reverts commit 91f2c1334571893d8f73527f2ccdb97e78923b9d, reversing
changes made to 4fdf5506972101623ad9d0e54e2ac67a81aab99d.
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies.xlsx
@@ -101,7 +101,7 @@
     <t xml:space="preserve">Tropical</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-07-16</t>
+    <t xml:space="preserve">16/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">MFE</t>
@@ -158,7 +158,7 @@
     <t xml:space="preserve">MR</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-07-19</t>
+    <t xml:space="preserve">19/07/2022</t>
   </si>
   <si>
     <t xml:space="preserve">Euploea darchia</t>
@@ -182,7 +182,7 @@
     <t xml:space="preserve">Subtropical</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-09-24</t>
+    <t xml:space="preserve">24/09/2022</t>
   </si>
   <si>
     <t xml:space="preserve">CI</t>

</xml_diff>

<commit_message>
Re-commit handling of dates in ISO 8601 format
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/repo/Oz_butterflies.xlsx
+++ b/tests/testthat/testdata/repo/Oz_butterflies.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -101,9 +101,6 @@
     <t xml:space="preserve">Tropical</t>
   </si>
   <si>
-    <t xml:space="preserve">16/07/2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">MFE</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t xml:space="preserve">MR</t>
   </si>
   <si>
-    <t xml:space="preserve">19/07/2022</t>
-  </si>
-  <si>
     <t xml:space="preserve">Euploea darchia</t>
   </si>
   <si>
@@ -180,9 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">Subtropical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24/09/2022</t>
   </si>
   <si>
     <t xml:space="preserve">CI</t>
@@ -199,13 +190,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,8 +224,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,23 +631,23 @@
       <c r="O2" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="1" t="n">
+        <v>44758</v>
+      </c>
+      <c r="Q2" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>30</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" t="s">
         <v>31</v>
-      </c>
-      <c r="S2" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" t="s">
-        <v>25</v>
-      </c>
-      <c r="U2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -661,13 +658,13 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
@@ -699,23 +696,23 @@
       <c r="O3" t="s">
         <v>28</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="1" t="n">
+        <v>44758</v>
+      </c>
+      <c r="Q3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" t="s">
-        <v>30</v>
-      </c>
       <c r="R3" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" t="s">
+        <v>25</v>
+      </c>
+      <c r="T3" t="s">
+        <v>25</v>
+      </c>
+      <c r="U3" t="s">
         <v>36</v>
-      </c>
-      <c r="S3" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" t="s">
-        <v>25</v>
-      </c>
-      <c r="U3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="4">
@@ -726,13 +723,13 @@
         <v>21</v>
       </c>
       <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>34</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
       </c>
       <c r="F4" t="s">
         <v>25</v>
@@ -764,23 +761,23 @@
       <c r="O4" t="s">
         <v>28</v>
       </c>
-      <c r="P4" t="s">
+      <c r="P4" s="1" t="n">
+        <v>44758</v>
+      </c>
+      <c r="Q4" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" t="s">
-        <v>30</v>
-      </c>
       <c r="R4" t="s">
+        <v>35</v>
+      </c>
+      <c r="S4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" t="s">
+        <v>25</v>
+      </c>
+      <c r="U4" t="s">
         <v>36</v>
-      </c>
-      <c r="S4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5">
@@ -791,10 +788,10 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="s">
         <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -818,7 +815,7 @@
         <v>25</v>
       </c>
       <c r="L5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M5" t="n">
         <v>-16.81425603</v>
@@ -829,14 +826,14 @@
       <c r="O5" t="s">
         <v>28</v>
       </c>
-      <c r="P5" t="s">
-        <v>29</v>
+      <c r="P5" s="1" t="n">
+        <v>44758</v>
       </c>
       <c r="Q5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R5" t="s">
         <v>41</v>
-      </c>
-      <c r="R5" t="s">
-        <v>42</v>
       </c>
       <c r="S5" t="s">
         <v>26</v>
@@ -845,7 +842,7 @@
         <v>26</v>
       </c>
       <c r="U5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6">
@@ -853,13 +850,13 @@
         <v>551</v>
       </c>
       <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>24</v>
@@ -883,7 +880,7 @@
         <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M6" t="n">
         <v>-16.45193583</v>
@@ -894,14 +891,14 @@
       <c r="O6" t="s">
         <v>28</v>
       </c>
-      <c r="P6" t="s">
-        <v>48</v>
+      <c r="P6" s="1" t="n">
+        <v>44761</v>
       </c>
       <c r="Q6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S6" t="s">
         <v>26</v>
@@ -910,7 +907,7 @@
         <v>26</v>
       </c>
       <c r="U6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7">
@@ -918,37 +915,37 @@
         <v>1361</v>
       </c>
       <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
         <v>51</v>
       </c>
-      <c r="C7" t="s">
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" t="s">
-        <v>54</v>
       </c>
       <c r="M7" t="n">
         <v>-27.344776</v>
@@ -957,25 +954,25 @@
         <v>153.0390842</v>
       </c>
       <c r="O7" t="s">
+        <v>53</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>44828</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>54</v>
+      </c>
+      <c r="R7" t="s">
         <v>55</v>
       </c>
-      <c r="P7" t="s">
+      <c r="S7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U7" t="s">
         <v>56</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>57</v>
-      </c>
-      <c r="R7" t="s">
-        <v>58</v>
-      </c>
-      <c r="S7" t="s">
-        <v>25</v>
-      </c>
-      <c r="T7" t="s">
-        <v>25</v>
-      </c>
-      <c r="U7" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>